<commit_message>
database fix and detailed product done
</commit_message>
<xml_diff>
--- a/PHP/Website Diogo HW/database/database.xlsx
+++ b/PHP/Website Diogo HW/database/database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GitHub\Everything-Diogo\PHP\Website Diogo HW\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D037F7E-8132-4AC2-96BE-4A965FDCC656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47BB54D-E85A-4A16-AA16-9BB729C61152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6E0C575C-11B3-4460-940E-EC104D05806F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E0C575C-11B3-4460-940E-EC104D05806F}"/>
   </bookViews>
   <sheets>
     <sheet name="database" sheetId="2" r:id="rId1"/>
@@ -451,9 +451,6 @@
     <t xml:space="preserve">       https://www.ldlc.com/fr-lu/fiche/PB00258881.html        </t>
   </si>
   <si>
-    <t>The Crucial P1 1TB SSD gives you massive storage capacity combined with NVMe PCIe technology to turn your PC into a blazing fast machine. With read and write speeds of up to 2000MB / s and 1700MB / s, you'll never have to wait.</t>
-  </si>
-  <si>
     <t>Crucial P1 M.2 PCIe NVMe 1 TB</t>
   </si>
   <si>
@@ -634,9 +631,6 @@
     <t xml:space="preserve">       https://www.ldlc.com/fr-lu/fiche/PB00316572.html        </t>
   </si>
   <si>
-    <t>The Cooler Master MasterCase H500 case has a special feature that will not leave you indifferent. Indeed, it is "The case" of the moment that gives you the choice of its design. It gives you the opportunity to opt for a tempered glass front panel or a mesh panel.</t>
-  </si>
-  <si>
     <t>Cooler Master MasterCase H500 Gris ARGB</t>
   </si>
   <si>
@@ -814,9 +808,6 @@
     <t xml:space="preserve">       https://www.ldlc.com/fr-lu/fiche/PB00250971.html        </t>
   </si>
   <si>
-    <t>Corsair's Vengeance RGB PRO Series high-end PC memories offer the best performance and stability for next-generation platforms with high overclocking potential.</t>
-  </si>
-  <si>
     <t>Corsair Vengeance RGB PRO Series</t>
   </si>
   <si>
@@ -1000,9 +991,6 @@
     <t xml:space="preserve">       https://www.ldlc.com/fr-lu/fiche/PB00263063.html        </t>
   </si>
   <si>
-    <t>Cooler Master's COSMOS C700P case is ready to accommodate a high-end configuration with Mini-ITX, Micro-ATX, ATX and E-ATX compatibility.</t>
-  </si>
-  <si>
     <t>Cooler Master COSMOS C700M</t>
   </si>
   <si>
@@ -1255,9 +1243,6 @@
     <t xml:space="preserve">       https://www.ldlc.com/fr-lu/fiche/PB00273079.html        </t>
   </si>
   <si>
-    <t>Choose a robust, scalable and high-performance solution with the Seagate IronWolf Pro 16TB hard drive. Designed for 1- to 24-bay business NAS, this 3.5 "drive is capable of supporting a workload of multi-user environments. up to 300 TB / year.</t>
-  </si>
-  <si>
     <t>Seagate IronWolf Pro</t>
   </si>
   <si>
@@ -1318,9 +1303,6 @@
     <t xml:space="preserve">       https://www.ldlc.com/fr-lu/fiche/PB00250525.html        </t>
   </si>
   <si>
-    <t>Exceptional in every way, the Corsair Obsidian 1000D "super tour" case benefits from a sublime design and ultra-advanced features. It has the incredible ability to host two systems simultaneously and has fully controllable RGB lighting.</t>
-  </si>
-  <si>
     <t>Corsair Obsidian 1000D</t>
   </si>
   <si>
@@ -1358,6 +1340,24 @@
   </si>
   <si>
     <t>ACERCA DE</t>
+  </si>
+  <si>
+    <t>The Crucial P1 1TB SSD gives you massive storage capacity combined with NVMe PCIe technology to turn your PC into a blazing fast machine. With read and write speeds of up to 2000MB / s and 1700MB / s, you ll never have to wait.</t>
+  </si>
+  <si>
+    <t>Corsair s Vengeance RGB PRO Series high-end PC memories offer the best performance and stability for next-generation platforms with high overclocking potential.</t>
+  </si>
+  <si>
+    <t>Cooler Master s COSMOS C700P case is ready to accommodate a high-end configuration with Mini-ITX, Micro-ATX, ATX and E-ATX compatibility.</t>
+  </si>
+  <si>
+    <t>The Cooler Master MasterCase H500 case has a special feature that will not leave you indifferent. Indeed, it is  The case  of the moment that gives you the choice of its design. It gives you the opportunity to opt for a tempered glass front panel or a mesh panel.</t>
+  </si>
+  <si>
+    <t>Choose a robust, scalable and high-performance solution with the Seagate IronWolf Pro 16TB hard drive. Designed for 1- to 24-bay business NAS, this 3.5  drive is capable of supporting a workload of multi-user environments. up to 300 TB / year.</t>
+  </si>
+  <si>
+    <t>Exceptional in every way, the Corsair Obsidian 1000D  super tour  case benefits from a sublime design and ultra-advanced features. It has the incredible ability to host two systems simultaneously and has fully controllable RGB lighting.</t>
   </si>
 </sst>
 </file>
@@ -1555,7 +1555,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1853,38 +1853,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2833D88C-1259-4C1C-ACBB-3401EECA7152}">
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="51.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="43.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="40.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1961,7 +1963,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -2038,7 +2040,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>46</v>
       </c>
@@ -2115,7 +2117,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>64</v>
       </c>
@@ -2192,7 +2194,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>84</v>
       </c>
@@ -2269,7 +2271,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>104</v>
       </c>
@@ -2346,7 +2348,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>125</v>
       </c>
@@ -2381,117 +2383,117 @@
         <v>144</v>
       </c>
       <c r="L7" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="V7" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="W7" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="W7" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="X7" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y7" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="K8">
         <v>100</v>
       </c>
       <c r="L8" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="T8" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="U8" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="V8" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="W8" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="X8" s="1" t="s">
         <v>83</v>
@@ -2500,178 +2502,178 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="K9">
         <v>126</v>
       </c>
       <c r="L9" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="S9" s="1" t="s">
+      <c r="T9" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="V9" s="1" t="s">
         <v>102</v>
       </c>
       <c r="W9" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="X9" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="Y9" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>111</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K10">
         <v>134</v>
       </c>
       <c r="L10" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="Q10" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="S10" s="1" t="s">
         <v>64</v>
       </c>
       <c r="T10" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="V10" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="W10" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="X10" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="X10" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="Y10" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>31</v>
@@ -2680,25 +2682,25 @@
         <v>32</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K11">
         <v>449</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>37</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>39</v>
@@ -2713,10 +2715,10 @@
         <v>40</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="V11" s="1" t="s">
         <v>37</v>
@@ -2728,27 +2730,27 @@
         <v>41</v>
       </c>
       <c r="Y11" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>31</v>
@@ -2757,19 +2759,19 @@
         <v>52</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K12">
         <v>849</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>57</v>
@@ -2781,19 +2783,19 @@
         <v>37</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>60</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="T12" s="1" t="s">
         <v>62</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="V12" s="1" t="s">
         <v>57</v>
@@ -2808,24 +2810,24 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>31</v>
@@ -2834,34 +2836,34 @@
         <v>70</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K13">
         <v>279</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>75</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>77</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S13" s="1" t="s">
         <v>80</v>
@@ -2870,7 +2872,7 @@
         <v>81</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="V13" s="1" t="s">
         <v>75</v>
@@ -2885,24 +2887,24 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>31</v>
@@ -2911,43 +2913,43 @@
         <v>90</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="K14">
         <v>241</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>255</v>
+        <v>432</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>95</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>97</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>37</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="V14" s="1" t="s">
         <v>102</v>
@@ -2959,27 +2961,27 @@
         <v>37</v>
       </c>
       <c r="Y14" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>268</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>31</v>
@@ -2988,43 +2990,43 @@
         <v>110</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="K15">
         <v>179</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>115</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>117</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="R15" s="1" t="s">
         <v>119</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="T15" s="1" t="s">
         <v>100</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="V15" s="1" t="s">
         <v>122</v>
@@ -3039,24 +3041,24 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>281</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>31</v>
@@ -3065,126 +3067,126 @@
         <v>131</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="K16">
         <v>107</v>
       </c>
       <c r="L16" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q16" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="R16" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="U16" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="N16" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="S16" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="T16" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="U16" s="1" t="s">
-        <v>288</v>
-      </c>
       <c r="V16" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="W16" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="W16" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="X16" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>290</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="K17">
         <v>127</v>
       </c>
       <c r="L17" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="T17" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="U17" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="N17" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="R17" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="S17" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="T17" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="U17" s="1" t="s">
-        <v>300</v>
-      </c>
       <c r="V17" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="W17" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="W17" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="X17" s="1" t="s">
         <v>83</v>
@@ -3193,178 +3195,178 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>305</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="K18">
         <v>139</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="N18" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="O18" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="Q18" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="Q18" s="1" t="s">
+      <c r="R18" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="R18" s="1" t="s">
+      <c r="S18" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="S18" s="1" t="s">
+      <c r="T18" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="T18" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="U18" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="V18" s="1" t="s">
         <v>102</v>
       </c>
       <c r="W18" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="X18" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="X18" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="Y18" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>315</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>111</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="K19">
         <v>479</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>317</v>
+        <v>433</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="N19" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="P19" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="O19" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="P19" s="1" t="s">
+      <c r="Q19" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="R19" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="S19" s="1" t="s">
         <v>84</v>
       </c>
       <c r="T19" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="V19" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="U19" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="V19" s="1" t="s">
+      <c r="W19" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="X19" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="W19" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="X19" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="Y19" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>31</v>
@@ -3376,22 +3378,22 @@
         <v>33</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="K20">
         <v>899</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>37</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="P20" s="1" t="s">
         <v>39</v>
@@ -3403,13 +3405,13 @@
         <v>41</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="V20" s="1" t="s">
         <v>37</v>
@@ -3421,27 +3423,27 @@
         <v>41</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>339</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>31</v>
@@ -3450,31 +3452,31 @@
         <v>52</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="K21">
         <v>1479</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>57</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="R21" s="1" t="s">
         <v>60</v>
@@ -3486,7 +3488,7 @@
         <v>62</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="V21" s="1" t="s">
         <v>57</v>
@@ -3501,24 +3503,24 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>352</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>31</v>
@@ -3527,19 +3529,19 @@
         <v>70</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="K22">
         <v>849</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>75</v>
@@ -3551,10 +3553,10 @@
         <v>77</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S22" s="1" t="s">
         <v>80</v>
@@ -3563,7 +3565,7 @@
         <v>81</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="V22" s="1" t="s">
         <v>57</v>
@@ -3575,24 +3577,24 @@
         <v>60</v>
       </c>
       <c r="Y22" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>359</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>363</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>89</v>
@@ -3604,31 +3606,31 @@
         <v>90</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="K23">
         <v>1039</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>95</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="P23" s="1" t="s">
         <v>97</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="R23" s="1" t="s">
         <v>37</v>
@@ -3637,10 +3639,10 @@
         <v>99</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="V23" s="1" t="s">
         <v>102</v>
@@ -3652,27 +3654,27 @@
         <v>37</v>
       </c>
       <c r="Y23" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>31</v>
@@ -3684,40 +3686,40 @@
         <v>111</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="K24">
         <v>199</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>115</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>117</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="R24" s="1" t="s">
         <v>119</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="T24" s="1" t="s">
         <v>100</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="V24" s="1" t="s">
         <v>122</v>
@@ -3729,27 +3731,27 @@
         <v>124</v>
       </c>
       <c r="Y24" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>389</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>31</v>
@@ -3758,318 +3760,318 @@
         <v>131</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="K25">
         <v>599</v>
       </c>
       <c r="L25" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="S25" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q25" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="S25" s="1" t="s">
-        <v>395</v>
-      </c>
       <c r="T25" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="V25" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="W25" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="W25" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="X25" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y25" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>400</v>
-      </c>
       <c r="F26" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="K26">
         <v>655</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>402</v>
+        <v>435</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="N26" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="O26" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="O26" s="1" t="s">
+      <c r="P26" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="P26" s="1" t="s">
+      <c r="Q26" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="Q26" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="R26" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="T26" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="V26" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="W26" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="W26" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="X26" s="1" t="s">
         <v>83</v>
       </c>
       <c r="Y26" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>410</v>
-      </c>
       <c r="F27" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="K27">
         <v>599</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="R27" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="S27" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="S27" s="1" t="s">
+      <c r="T27" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="T27" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="U27" s="1" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="V27" s="1" t="s">
         <v>102</v>
       </c>
       <c r="W27" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="X27" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="X27" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="Y27" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="K28">
         <v>599</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>423</v>
+        <v>436</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="N28" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="P28" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="O28" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="P28" s="1" t="s">
+      <c r="Q28" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="R28" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="Q28" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="S28" s="1" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="T28" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="U28" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="V28" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="U28" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="V28" s="1" t="s">
+      <c r="W28" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="X28" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="W28" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="X28" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="Y28" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="I29" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="J29" s="1" t="s">
         <v>430</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>436</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>45</v>
@@ -4128,7 +4130,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>